<commit_message>
GDE-8209 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S4_EU_NonRPA_Branch.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S4_EU_NonRPA_Branch.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="923" firstSheet="3" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED02_FacilitySetup" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED08_OngoingFeeSetup" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SYND02_PrimaryAllocation" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CRED07_UpfrontFee_Payment" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV01_LoanDrawdown" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH06_PricingChangeTransaction" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DLCH01_DealChangeTransaction" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV18_Payments" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV21_InterestPayments" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SERV29_PaymentFees" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMCH04_DealChangeTransaction" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRPO12_PortfolioSettledDisc" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -34,7 +35,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -145,6 +146,11 @@
       <family val="2"/>
       <b val="1"/>
       <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -281,12 +287,12 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -423,6 +429,17 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="15" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,6 +1393,519 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AR5"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="6.140625" customWidth="1" style="15" min="1" max="1"/>
+    <col width="39.28515625" customWidth="1" style="15" min="2" max="2"/>
+    <col width="18.7109375" customWidth="1" style="15" min="3" max="3"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
+    <col width="16.28515625" customWidth="1" style="15" min="5" max="5"/>
+    <col width="21.140625" customWidth="1" style="15" min="6" max="6"/>
+    <col width="14.5703125" customWidth="1" style="15" min="7" max="7"/>
+    <col width="26.7109375" customWidth="1" style="15" min="8" max="8"/>
+    <col width="33.28515625" customWidth="1" style="15" min="9" max="9"/>
+    <col width="21.7109375" customWidth="1" style="15" min="10" max="10"/>
+    <col width="17.42578125" customWidth="1" style="15" min="11" max="11"/>
+    <col width="21.140625" customWidth="1" style="15" min="12" max="12"/>
+    <col width="10.42578125" customWidth="1" style="15" min="13" max="13"/>
+    <col width="18.5703125" customWidth="1" style="15" min="14" max="14"/>
+    <col width="14.140625" customWidth="1" style="15" min="15" max="15"/>
+    <col width="23.28515625" customWidth="1" style="15" min="16" max="16"/>
+    <col width="17.28515625" customWidth="1" style="15" min="17" max="17"/>
+    <col width="18.42578125" customWidth="1" style="15" min="18" max="18"/>
+    <col width="18.28515625" customWidth="1" style="15" min="19" max="19"/>
+    <col width="24.140625" customWidth="1" style="15" min="20" max="20"/>
+    <col width="23" customWidth="1" style="15" min="21" max="21"/>
+    <col width="20.5703125" customWidth="1" style="15" min="22" max="22"/>
+    <col width="18.7109375" customWidth="1" style="15" min="23" max="23"/>
+    <col width="30.28515625" customWidth="1" style="15" min="24" max="24"/>
+    <col width="27.7109375" customWidth="1" style="15" min="25" max="25"/>
+    <col width="22.85546875" customWidth="1" style="15" min="26" max="26"/>
+    <col width="26.85546875" customWidth="1" style="15" min="27" max="27"/>
+    <col width="21" customWidth="1" style="15" min="28" max="28"/>
+    <col width="28" customWidth="1" style="15" min="29" max="29"/>
+    <col width="21.42578125" customWidth="1" style="15" min="30" max="30"/>
+    <col width="32.28515625" customWidth="1" style="15" min="31" max="31"/>
+    <col width="36.5703125" customWidth="1" style="15" min="32" max="32"/>
+    <col width="16.5703125" customWidth="1" style="15" min="33" max="33"/>
+    <col width="24.28515625" customWidth="1" style="15" min="34" max="34"/>
+    <col width="15.7109375" customWidth="1" style="15" min="35" max="35"/>
+    <col width="22.140625" customWidth="1" style="15" min="36" max="36"/>
+    <col width="18.140625" customWidth="1" style="15" min="37" max="37"/>
+    <col width="14.85546875" customWidth="1" style="15" min="38" max="38"/>
+    <col width="22.85546875" customWidth="1" style="15" min="39" max="39"/>
+    <col width="20.5703125" customWidth="1" style="15" min="40" max="41"/>
+    <col width="40.85546875" customWidth="1" style="86" min="42" max="42"/>
+    <col width="14.7109375" customWidth="1" style="86" min="43" max="43"/>
+    <col width="12.140625" bestFit="1" customWidth="1" min="44" max="44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="29" t="inlineStr">
+        <is>
+          <t>rowid</t>
+        </is>
+      </c>
+      <c r="B1" s="12" t="inlineStr">
+        <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="29" t="inlineStr">
+        <is>
+          <t>Contact_Email</t>
+        </is>
+      </c>
+      <c r="D1" s="30" t="inlineStr">
+        <is>
+          <t>Deal_Name</t>
+        </is>
+      </c>
+      <c r="E1" s="29" t="inlineStr">
+        <is>
+          <t>Facility_Currency</t>
+        </is>
+      </c>
+      <c r="F1" s="30" t="inlineStr">
+        <is>
+          <t>Facility_Name</t>
+        </is>
+      </c>
+      <c r="G1" s="29" t="inlineStr">
+        <is>
+          <t>Facility_Spread</t>
+        </is>
+      </c>
+      <c r="H1" s="29" t="inlineStr">
+        <is>
+          <t>Facility_CurrentAvailToDraw</t>
+        </is>
+      </c>
+      <c r="I1" s="29" t="inlineStr">
+        <is>
+          <t>Facility_CurrentGlobalOutstandings</t>
+        </is>
+      </c>
+      <c r="J1" s="30" t="inlineStr">
+        <is>
+          <t>Borrower1_ShortName</t>
+        </is>
+      </c>
+      <c r="K1" s="29" t="inlineStr">
+        <is>
+          <t>Outstanding_Type</t>
+        </is>
+      </c>
+      <c r="L1" s="30" t="inlineStr">
+        <is>
+          <t>Loan_FacilityName</t>
+        </is>
+      </c>
+      <c r="M1" s="30" t="inlineStr">
+        <is>
+          <t>Loan_Alias</t>
+        </is>
+      </c>
+      <c r="N1" s="29" t="inlineStr">
+        <is>
+          <t>Loan_PricingOption</t>
+        </is>
+      </c>
+      <c r="O1" s="29" t="inlineStr">
+        <is>
+          <t>Loan_Currency</t>
+        </is>
+      </c>
+      <c r="P1" s="29" t="inlineStr">
+        <is>
+          <t>Loan_RequestedAmount</t>
+        </is>
+      </c>
+      <c r="Q1" s="29" t="inlineStr">
+        <is>
+          <t>HostBankSharePct</t>
+        </is>
+      </c>
+      <c r="R1" s="30" t="inlineStr">
+        <is>
+          <t>Loan_EffectiveDate</t>
+        </is>
+      </c>
+      <c r="S1" s="30" t="inlineStr">
+        <is>
+          <t>Loan_MaturityDate</t>
+        </is>
+      </c>
+      <c r="T1" s="29" t="inlineStr">
+        <is>
+          <t>Loan_RepricingFrequency</t>
+        </is>
+      </c>
+      <c r="U1" s="29" t="inlineStr">
+        <is>
+          <t>Loan_IntCycleFrequency</t>
+        </is>
+      </c>
+      <c r="V1" s="29" t="inlineStr">
+        <is>
+          <t>Loan_Accrue</t>
+        </is>
+      </c>
+      <c r="W1" s="29" t="inlineStr">
+        <is>
+          <t>Borrower_BaseRate</t>
+        </is>
+      </c>
+      <c r="X1" s="29" t="inlineStr">
+        <is>
+          <t>Repayment_ScheduleFrequency</t>
+        </is>
+      </c>
+      <c r="Y1" s="29" t="inlineStr">
+        <is>
+          <t>Repayment_NumberOfCycles</t>
+        </is>
+      </c>
+      <c r="Z1" s="30" t="inlineStr">
+        <is>
+          <t>Repayment_TriggerDate</t>
+        </is>
+      </c>
+      <c r="AA1" s="29" t="inlineStr">
+        <is>
+          <t>Repayment_NonBusDayRule</t>
+        </is>
+      </c>
+      <c r="AB1" s="2" t="inlineStr">
+        <is>
+          <t>WIP_TransactionType</t>
+        </is>
+      </c>
+      <c r="AC1" s="2" t="inlineStr">
+        <is>
+          <t>WIP_AwaitingApprovalStatus</t>
+        </is>
+      </c>
+      <c r="AD1" s="2" t="inlineStr">
+        <is>
+          <t>WIP_OutstandingType</t>
+        </is>
+      </c>
+      <c r="AE1" s="2" t="inlineStr">
+        <is>
+          <t>WIP_AwaitingRateApprovalStatus</t>
+        </is>
+      </c>
+      <c r="AF1" s="2" t="inlineStr">
+        <is>
+          <t>WIP_AwaitingReleaseCashflowsStatus</t>
+        </is>
+      </c>
+      <c r="AG1" s="2" t="inlineStr">
+        <is>
+          <t>Borrower_Profile</t>
+        </is>
+      </c>
+      <c r="AH1" s="13" t="inlineStr">
+        <is>
+          <t>LIQCustomer_ShortName</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="inlineStr">
+        <is>
+          <t>LIQCustomer_ID</t>
+        </is>
+      </c>
+      <c r="AJ1" s="2" t="inlineStr">
+        <is>
+          <t>Remittance_Instruction</t>
+        </is>
+      </c>
+      <c r="AK1" s="2" t="inlineStr">
+        <is>
+          <t>Remittance_Status</t>
+        </is>
+      </c>
+      <c r="AL1" s="2" t="inlineStr">
+        <is>
+          <t>Loan_Currency</t>
+        </is>
+      </c>
+      <c r="AM1" s="13" t="inlineStr">
+        <is>
+          <t>Remittance_Description</t>
+        </is>
+      </c>
+      <c r="AN1" s="2" t="inlineStr">
+        <is>
+          <t>HostBank_GLAccount</t>
+        </is>
+      </c>
+      <c r="AO1" s="2" t="inlineStr">
+        <is>
+          <t>Borrower_GLAccount</t>
+        </is>
+      </c>
+      <c r="AP1" s="2" t="inlineStr">
+        <is>
+          <t>Host_Bank</t>
+        </is>
+      </c>
+      <c r="AQ1" s="2" t="inlineStr">
+        <is>
+          <t>NoticeStatus</t>
+        </is>
+      </c>
+      <c r="AR1" s="2" t="inlineStr">
+        <is>
+          <t>BranchCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="86">
+      <c r="A2" s="86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="86" t="inlineStr">
+        <is>
+          <t>EVG_PTYLIQ01 Scenario1 Baseline Bilateral</t>
+        </is>
+      </c>
+      <c r="C2" s="31" t="inlineStr">
+        <is>
+          <t>john.blogg@abc.com</t>
+        </is>
+      </c>
+      <c r="D2" s="86" t="inlineStr">
+        <is>
+          <t>NON RPA HB BRANCH 20M_20102020150220NIP</t>
+        </is>
+      </c>
+      <c r="E2" s="15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="F2" s="86" t="inlineStr">
+        <is>
+          <t>CEU_FAC_10062020130642XHO</t>
+        </is>
+      </c>
+      <c r="G2" s="15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H2" s="86" t="inlineStr">
+        <is>
+          <t>100,000.00</t>
+        </is>
+      </c>
+      <c r="I2" s="86" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="J2" s="86" t="inlineStr">
+        <is>
+          <t>SHORTNME2255</t>
+        </is>
+      </c>
+      <c r="K2" s="15" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="L2" s="86" t="inlineStr">
+        <is>
+          <t>CEU_FAC_10062020130642XHO</t>
+        </is>
+      </c>
+      <c r="M2" s="86" t="inlineStr">
+        <is>
+          <t>60000278</t>
+        </is>
+      </c>
+      <c r="N2" s="15" t="inlineStr">
+        <is>
+          <t>Fixed Rate Option</t>
+        </is>
+      </c>
+      <c r="O2" s="15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="P2" s="15" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="Q2" s="15" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="R2" s="86" t="inlineStr">
+        <is>
+          <t>25-May-2020</t>
+        </is>
+      </c>
+      <c r="S2" s="86" t="inlineStr">
+        <is>
+          <t>26-May-2025</t>
+        </is>
+      </c>
+      <c r="T2" s="15" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="U2" s="15" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="V2" s="15" t="inlineStr">
+        <is>
+          <t>to the actual due date</t>
+        </is>
+      </c>
+      <c r="W2" s="15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="X2" s="15" t="inlineStr">
+        <is>
+          <t>Weeks</t>
+        </is>
+      </c>
+      <c r="Y2" s="15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Z2" s="86" t="inlineStr">
+        <is>
+          <t>25-May-2020</t>
+        </is>
+      </c>
+      <c r="AA2" s="15" t="inlineStr">
+        <is>
+          <t>Next Business Day</t>
+        </is>
+      </c>
+      <c r="AB2" s="86" t="inlineStr">
+        <is>
+          <t>Outstandings</t>
+        </is>
+      </c>
+      <c r="AC2" s="86" t="inlineStr">
+        <is>
+          <t>Awaiting Approval</t>
+        </is>
+      </c>
+      <c r="AD2" s="86" t="inlineStr">
+        <is>
+          <t>Loan Initial Drawdown</t>
+        </is>
+      </c>
+      <c r="AE2" s="15" t="inlineStr">
+        <is>
+          <t>Awaiting Rate Approval</t>
+        </is>
+      </c>
+      <c r="AF2" s="15" t="inlineStr">
+        <is>
+          <t>Awaiting Release Cashflows</t>
+        </is>
+      </c>
+      <c r="AG2" s="15" t="inlineStr">
+        <is>
+          <t>Borrower</t>
+        </is>
+      </c>
+      <c r="AH2" s="86" t="inlineStr">
+        <is>
+          <t>SHORTNME2255</t>
+        </is>
+      </c>
+      <c r="AI2" s="86" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="AJ2" s="86" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="AK2" s="86" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="AL2" s="86" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="AM2" s="86" t="inlineStr">
+        <is>
+          <t>IMTEUR1-0902</t>
+        </is>
+      </c>
+      <c r="AN2" s="32" t="inlineStr">
+        <is>
+          <t>12001001836</t>
+        </is>
+      </c>
+      <c r="AO2" s="32" t="inlineStr">
+        <is>
+          <t>18567000000</t>
+        </is>
+      </c>
+      <c r="AP2" s="86" t="inlineStr">
+        <is>
+          <t>CG852/Hold for Investment - Europe/BP_CML</t>
+        </is>
+      </c>
+      <c r="AQ2" s="86" t="inlineStr">
+        <is>
+          <t>Awaiting release</t>
+        </is>
+      </c>
+      <c r="AR2" s="86" t="inlineStr">
+        <is>
+          <t>CG852</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="AP5" s="33" t="n"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1853,7 +2383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1944,7 +2474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2405,7 +2935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2924,7 +3454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3379,7 +3909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3470,7 +4000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3498,8 +4028,8 @@
     <col width="21.5703125" bestFit="1" customWidth="1" style="88" min="13" max="13"/>
     <col width="19.140625" bestFit="1" customWidth="1" style="88" min="14" max="14"/>
     <col width="32.7109375" bestFit="1" customWidth="1" style="88" min="15" max="15"/>
-    <col width="8.7109375" customWidth="1" style="88" min="16" max="18"/>
-    <col width="8.7109375" customWidth="1" style="88" min="19" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="88" min="16" max="21"/>
+    <col width="8.7109375" customWidth="1" style="88" min="22" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="89">
@@ -3714,8 +4244,8 @@
     <col width="8.7109375" customWidth="1" style="64" min="42" max="42"/>
     <col width="11.28515625" customWidth="1" style="64" min="43" max="43"/>
     <col width="8.7109375" customWidth="1" style="64" min="44" max="45"/>
-    <col width="9.140625" customWidth="1" style="68" min="46" max="66"/>
-    <col width="9.140625" customWidth="1" style="68" min="67" max="16384"/>
+    <col width="9.140625" customWidth="1" style="68" min="46" max="69"/>
+    <col width="9.140625" customWidth="1" style="68" min="70" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="61">
@@ -6407,8 +6937,8 @@
   <dimension ref="A1:CY2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" topLeftCell="BR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BR16" sqref="BR16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7401,7 +7931,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G3" sqref="G3"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -7884,7 +8414,7 @@
   </sheetPr>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -8169,46 +8699,62 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor theme="9" tint="0.3999755851924192"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="6.140625" customWidth="1" style="86" min="1" max="1"/>
-    <col width="39.28515625" customWidth="1" style="86" min="2" max="2"/>
-    <col width="46.28515625" customWidth="1" style="86" min="3" max="3"/>
-    <col width="34.5703125" bestFit="1" customWidth="1" style="86" min="4" max="4"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="86" min="5" max="5"/>
-    <col width="21" customWidth="1" style="86" min="6" max="6"/>
-    <col width="17.7109375" customWidth="1" style="86" min="7" max="7"/>
-    <col width="25" bestFit="1" customWidth="1" style="86" min="8" max="8"/>
-    <col width="26.28515625" customWidth="1" style="86" min="9" max="9"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="86" min="1" max="1"/>
+    <col width="28" bestFit="1" customWidth="1" style="86" min="2" max="2"/>
+    <col width="44.140625" bestFit="1" customWidth="1" style="86" min="3" max="3"/>
+    <col width="31.140625" bestFit="1" customWidth="1" style="86" min="4" max="4"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="86" min="5" max="5"/>
+    <col width="22" bestFit="1" customWidth="1" style="86" min="6" max="6"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="86" min="7" max="7"/>
+    <col width="26.140625" bestFit="1" customWidth="1" style="86" min="8" max="8"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" style="86" min="9" max="9"/>
     <col width="19.42578125" customWidth="1" style="86" min="10" max="10"/>
-    <col width="21.140625" customWidth="1" style="86" min="11" max="12"/>
-    <col width="18.140625" customWidth="1" style="86" min="13" max="13"/>
-    <col width="29.140625" customWidth="1" style="86" min="14" max="14"/>
-    <col width="17.5703125" customWidth="1" style="86" min="15" max="15"/>
-    <col width="26.28515625" customWidth="1" style="86" min="16" max="16"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" style="86" min="11" max="11"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" style="86" min="12" max="12"/>
+    <col width="19" bestFit="1" customWidth="1" style="86" min="13" max="13"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" style="86" min="14" max="14"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="86" min="15" max="15"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="86" min="16" max="16"/>
     <col width="40.7109375" bestFit="1" customWidth="1" style="86" min="17" max="17"/>
-    <col width="26.5703125" customWidth="1" style="86" min="18" max="18"/>
+    <col width="27" bestFit="1" customWidth="1" style="86" min="18" max="18"/>
     <col width="26.42578125" customWidth="1" style="86" min="19" max="19"/>
-    <col width="27.28515625" customWidth="1" style="86" min="20" max="20"/>
-    <col width="20" customWidth="1" style="86" min="21" max="21"/>
+    <col width="27.5703125" bestFit="1" customWidth="1" style="86" min="20" max="20"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="86" min="21" max="21"/>
     <col width="11.85546875" customWidth="1" style="86" min="22" max="22"/>
     <col width="40.7109375" bestFit="1" customWidth="1" style="86" min="23" max="23"/>
-    <col width="18.140625" customWidth="1" style="86" min="24" max="24"/>
-    <col width="12.7109375" customWidth="1" style="14" min="25" max="25"/>
-    <col width="11.140625" customWidth="1" style="14" min="26" max="26"/>
-    <col width="35.28515625" bestFit="1" customWidth="1" style="86" min="27" max="27"/>
-    <col width="31.140625" customWidth="1" style="86" min="28" max="28"/>
-    <col width="31.140625" bestFit="1" customWidth="1" min="29" max="29"/>
+    <col width="18.42578125" bestFit="1" customWidth="1" style="86" min="24" max="24"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="14" min="25" max="25"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" style="14" min="26" max="26"/>
+    <col width="28.85546875" bestFit="1" customWidth="1" style="86" min="27" max="27"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" style="86" min="28" max="28"/>
+    <col width="21.140625" bestFit="1" customWidth="1" min="29" max="29"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" min="30" max="30"/>
+    <col width="22" bestFit="1" customWidth="1" min="31" max="31"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" min="32" max="32"/>
+    <col width="26.140625" bestFit="1" customWidth="1" min="33" max="33"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" min="34" max="34"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" min="35" max="35"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" min="36" max="36"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" min="37" max="37"/>
+    <col width="19" bestFit="1" customWidth="1" min="38" max="38"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" min="39" max="39"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" min="40" max="40"/>
+    <col width="27" bestFit="1" customWidth="1" min="41" max="41"/>
+    <col width="40.7109375" bestFit="1" customWidth="1" min="42" max="42"/>
+    <col width="19.140625" bestFit="1" customWidth="1" min="43" max="43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customFormat="1" customHeight="1" s="1">
@@ -8234,17 +8780,17 @@
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>Primary_Lender</t>
+          <t>Primary_Lender1</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Primary_LenderLoc</t>
+          <t>Primary_LenderLoc1</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Primary_RiskBook</t>
+          <t>Primary_RiskBook1</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
@@ -8259,17 +8805,17 @@
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Primary_PctOfDeal</t>
+          <t>Primary_PctOfDeal1</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>BuySellPrice</t>
+          <t>Primary_BuySellPrice1</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>SellAmount</t>
+          <t>SellAmount1</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
@@ -8279,7 +8825,7 @@
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>Primary_Contact</t>
+          <t>Primary_Contact1</t>
         </is>
       </c>
       <c r="O1" s="2" t="inlineStr">
@@ -8289,12 +8835,12 @@
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>Primary_Portfolio</t>
+          <t>Primary_Portfolio1</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
         <is>
-          <t>Primary_PortfolioBranch</t>
+          <t>Primary_PortfolioBranch1</t>
         </is>
       </c>
       <c r="R1" s="2" t="inlineStr">
@@ -8355,6 +8901,76 @@
       <c r="AC1" s="6" t="inlineStr">
         <is>
           <t>AdminAgent_SGAlias</t>
+        </is>
+      </c>
+      <c r="AD1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_Lender2</t>
+        </is>
+      </c>
+      <c r="AE1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_LenderLoc2</t>
+        </is>
+      </c>
+      <c r="AF1" s="94" t="inlineStr">
+        <is>
+          <t>Primary_RiskBook2</t>
+        </is>
+      </c>
+      <c r="AG1" s="94" t="inlineStr">
+        <is>
+          <t>ExpenseCode_Description</t>
+        </is>
+      </c>
+      <c r="AH1" s="95" t="inlineStr">
+        <is>
+          <t>Primaries_TransactionType</t>
+        </is>
+      </c>
+      <c r="AI1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_PctOfDeal2</t>
+        </is>
+      </c>
+      <c r="AJ1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_BuySellPrice2</t>
+        </is>
+      </c>
+      <c r="AK1" s="2" t="inlineStr">
+        <is>
+          <t>SellAmount2</t>
+        </is>
+      </c>
+      <c r="AL1" s="94" t="inlineStr">
+        <is>
+          <t>Primary_Comment</t>
+        </is>
+      </c>
+      <c r="AM1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_Contact2</t>
+        </is>
+      </c>
+      <c r="AN1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_SGAlias2</t>
+        </is>
+      </c>
+      <c r="AO1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_Portfolio2</t>
+        </is>
+      </c>
+      <c r="AP1" s="2" t="inlineStr">
+        <is>
+          <t>Primary_PortfolioBranch2</t>
+        </is>
+      </c>
+      <c r="AQ1" s="2" t="inlineStr">
+        <is>
+          <t>Deal_ExpenseCode</t>
         </is>
       </c>
     </row>
@@ -8391,12 +9007,12 @@
       </c>
       <c r="G2" s="86" t="inlineStr">
         <is>
-          <t>IT_SAF</t>
+          <t>NR_PRF</t>
         </is>
       </c>
       <c r="H2" s="86" t="inlineStr">
         <is>
-          <t>Structured Asset Finance</t>
+          <t>Natural Resources &amp; Energy</t>
         </is>
       </c>
       <c r="I2" s="86" t="inlineStr">
@@ -8405,14 +9021,14 @@
         </is>
       </c>
       <c r="J2" s="86" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="K2" s="86" t="n">
         <v>100</v>
       </c>
       <c r="L2" s="46" t="inlineStr">
         <is>
-          <t>50,000,000.00</t>
+          <t>8,000,000.00</t>
         </is>
       </c>
       <c r="M2" s="86" t="inlineStr">
@@ -8442,44 +9058,44 @@
       </c>
       <c r="R2" s="5" t="inlineStr">
         <is>
+          <t>8,000,000.00</t>
+        </is>
+      </c>
+      <c r="S2" s="5" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="T2" s="86" t="inlineStr">
+        <is>
+          <t>26-May-2025</t>
+        </is>
+      </c>
+      <c r="U2" s="86" t="inlineStr">
+        <is>
+          <t>25-May-2020</t>
+        </is>
+      </c>
+      <c r="W2" s="86" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - Amsterdam</t>
+        </is>
+      </c>
+      <c r="X2" s="14" t="inlineStr">
+        <is>
           <t>100,000.00</t>
         </is>
       </c>
-      <c r="S2" s="5" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="T2" s="86" t="inlineStr">
-        <is>
-          <t>26-May-2025</t>
-        </is>
-      </c>
-      <c r="U2" s="86" t="inlineStr">
+      <c r="Y2" s="86" t="inlineStr">
         <is>
           <t>25-May-2020</t>
         </is>
       </c>
-      <c r="W2" s="86" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia - Amsterdam</t>
-        </is>
-      </c>
-      <c r="X2" s="14" t="inlineStr">
-        <is>
-          <t>100,000.00</t>
-        </is>
-      </c>
-      <c r="Y2" s="86" t="inlineStr">
+      <c r="Z2" s="86" t="inlineStr">
         <is>
           <t>25-May-2020</t>
         </is>
       </c>
-      <c r="Z2" s="86" t="inlineStr">
-        <is>
-          <t>25-May-2020</t>
-        </is>
-      </c>
       <c r="AA2" s="86" t="inlineStr">
         <is>
           <t>CBA AMSTERDAM</t>
@@ -8493,6 +9109,72 @@
       <c r="AC2" s="86" t="inlineStr">
         <is>
           <t>LOAN</t>
+        </is>
+      </c>
+      <c r="AD2" s="86" t="inlineStr">
+        <is>
+          <t>COMMONWEALTH BANK AU-OBU</t>
+        </is>
+      </c>
+      <c r="AE2" s="86" t="inlineStr">
+        <is>
+          <t>Sydney, NSW,Australia</t>
+        </is>
+      </c>
+      <c r="AF2" s="52" t="inlineStr">
+        <is>
+          <t>DM_CFS</t>
+        </is>
+      </c>
+      <c r="AG2" s="52" t="inlineStr">
+        <is>
+          <t>CFS General Warehouses</t>
+        </is>
+      </c>
+      <c r="AH2" s="52" t="inlineStr">
+        <is>
+          <t>Origination</t>
+        </is>
+      </c>
+      <c r="AI2" s="86" t="n">
+        <v>60</v>
+      </c>
+      <c r="AJ2" s="86" t="n">
+        <v>100</v>
+      </c>
+      <c r="AK2" s="46" t="inlineStr">
+        <is>
+          <t>12,000,000.00</t>
+        </is>
+      </c>
+      <c r="AL2" s="52" t="inlineStr">
+        <is>
+          <t>Add Comment</t>
+        </is>
+      </c>
+      <c r="AM2" s="5" t="inlineStr">
+        <is>
+          <t>Lending,${SPACE}${SPACE}Ops</t>
+        </is>
+      </c>
+      <c r="AN2" s="86" t="inlineStr">
+        <is>
+          <t>LENDING</t>
+        </is>
+      </c>
+      <c r="AO2" s="5" t="inlineStr">
+        <is>
+          <t>Hold for Investment - Australia</t>
+        </is>
+      </c>
+      <c r="AP2" s="86" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - OBU</t>
+        </is>
+      </c>
+      <c r="AQ2" s="86" t="inlineStr">
+        <is>
+          <t>NR_PRF</t>
         </is>
       </c>
     </row>
@@ -8782,508 +9464,196 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor theme="9" tint="0.3999755851924192"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR5"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" customWidth="1" style="15" min="1" max="1"/>
-    <col width="39.28515625" customWidth="1" style="15" min="2" max="2"/>
-    <col width="18.7109375" customWidth="1" style="15" min="3" max="3"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="15" min="4" max="4"/>
-    <col width="16.28515625" customWidth="1" style="15" min="5" max="5"/>
-    <col width="21.140625" customWidth="1" style="15" min="6" max="6"/>
-    <col width="14.5703125" customWidth="1" style="15" min="7" max="7"/>
-    <col width="26.7109375" customWidth="1" style="15" min="8" max="8"/>
-    <col width="33.28515625" customWidth="1" style="15" min="9" max="9"/>
-    <col width="21.7109375" customWidth="1" style="15" min="10" max="10"/>
-    <col width="17.42578125" customWidth="1" style="15" min="11" max="11"/>
-    <col width="21.140625" customWidth="1" style="15" min="12" max="12"/>
-    <col width="10.42578125" customWidth="1" style="15" min="13" max="13"/>
-    <col width="18.5703125" customWidth="1" style="15" min="14" max="14"/>
-    <col width="14.140625" customWidth="1" style="15" min="15" max="15"/>
-    <col width="23.28515625" customWidth="1" style="15" min="16" max="16"/>
-    <col width="17.28515625" customWidth="1" style="15" min="17" max="17"/>
-    <col width="18.42578125" customWidth="1" style="15" min="18" max="18"/>
-    <col width="18.28515625" customWidth="1" style="15" min="19" max="19"/>
-    <col width="24.140625" customWidth="1" style="15" min="20" max="20"/>
-    <col width="23" customWidth="1" style="15" min="21" max="21"/>
-    <col width="20.5703125" customWidth="1" style="15" min="22" max="22"/>
-    <col width="18.7109375" customWidth="1" style="15" min="23" max="23"/>
-    <col width="30.28515625" customWidth="1" style="15" min="24" max="24"/>
-    <col width="27.7109375" customWidth="1" style="15" min="25" max="25"/>
-    <col width="22.85546875" customWidth="1" style="15" min="26" max="26"/>
-    <col width="26.85546875" customWidth="1" style="15" min="27" max="27"/>
-    <col width="21" customWidth="1" style="15" min="28" max="28"/>
-    <col width="28" customWidth="1" style="15" min="29" max="29"/>
-    <col width="21.42578125" customWidth="1" style="15" min="30" max="30"/>
-    <col width="32.28515625" customWidth="1" style="15" min="31" max="31"/>
-    <col width="36.5703125" customWidth="1" style="15" min="32" max="32"/>
-    <col width="16.5703125" customWidth="1" style="15" min="33" max="33"/>
-    <col width="24.28515625" customWidth="1" style="15" min="34" max="34"/>
-    <col width="15.7109375" customWidth="1" style="15" min="35" max="35"/>
-    <col width="22.140625" customWidth="1" style="15" min="36" max="36"/>
-    <col width="18.140625" customWidth="1" style="15" min="37" max="37"/>
-    <col width="14.85546875" customWidth="1" style="15" min="38" max="38"/>
-    <col width="22.85546875" customWidth="1" style="15" min="39" max="39"/>
-    <col width="20.5703125" customWidth="1" style="15" min="40" max="41"/>
-    <col width="40.85546875" customWidth="1" style="86" min="42" max="42"/>
-    <col width="14.7109375" customWidth="1" style="86" min="43" max="43"/>
-    <col width="12.140625" bestFit="1" customWidth="1" min="44" max="44"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="98" min="1" max="1"/>
+    <col width="52" bestFit="1" customWidth="1" style="98" min="2" max="2"/>
+    <col width="44.140625" bestFit="1" customWidth="1" style="98" min="3" max="3"/>
+    <col width="20.140625" bestFit="1" customWidth="1" style="98" min="4" max="4"/>
+    <col width="26" bestFit="1" customWidth="1" style="98" min="5" max="5"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="98" min="6" max="6"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" style="98" min="7" max="7"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="98" min="8" max="8"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="98" min="9" max="9"/>
+    <col width="23.7109375" bestFit="1" customWidth="1" style="98" min="10" max="10"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" style="98" min="11" max="11"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="98" min="12" max="12"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" style="98" min="13" max="13"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="98" min="14" max="14"/>
+    <col width="34.140625" bestFit="1" customWidth="1" style="98" min="15" max="15"/>
+    <col width="6.140625" bestFit="1" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="1">
-      <c r="A1" s="29" t="inlineStr">
+    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="97" thickBot="1">
+      <c r="A1" s="24" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="12" t="inlineStr">
+      <c r="B1" s="24" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="29" t="inlineStr">
-        <is>
-          <t>Contact_Email</t>
-        </is>
-      </c>
-      <c r="D1" s="30" t="inlineStr">
+      <c r="C1" s="96" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="E1" s="29" t="inlineStr">
-        <is>
-          <t>Facility_Currency</t>
-        </is>
-      </c>
-      <c r="F1" s="30" t="inlineStr">
-        <is>
-          <t>Facility_Name</t>
-        </is>
-      </c>
-      <c r="G1" s="29" t="inlineStr">
-        <is>
-          <t>Facility_Spread</t>
-        </is>
-      </c>
-      <c r="H1" s="29" t="inlineStr">
-        <is>
-          <t>Facility_CurrentAvailToDraw</t>
-        </is>
-      </c>
-      <c r="I1" s="29" t="inlineStr">
-        <is>
-          <t>Facility_CurrentGlobalOutstandings</t>
-        </is>
-      </c>
-      <c r="J1" s="30" t="inlineStr">
-        <is>
-          <t>Borrower1_ShortName</t>
-        </is>
-      </c>
-      <c r="K1" s="29" t="inlineStr">
-        <is>
-          <t>Outstanding_Type</t>
-        </is>
-      </c>
-      <c r="L1" s="30" t="inlineStr">
-        <is>
-          <t>Loan_FacilityName</t>
-        </is>
-      </c>
-      <c r="M1" s="30" t="inlineStr">
-        <is>
-          <t>Loan_Alias</t>
-        </is>
-      </c>
-      <c r="N1" s="29" t="inlineStr">
-        <is>
-          <t>Loan_PricingOption</t>
-        </is>
-      </c>
-      <c r="O1" s="29" t="inlineStr">
+      <c r="D1" s="96" t="inlineStr">
+        <is>
+          <t>UpfrontFee_Amount</t>
+        </is>
+      </c>
+      <c r="E1" s="24" t="inlineStr">
+        <is>
+          <t>Fee_Type</t>
+        </is>
+      </c>
+      <c r="F1" s="24" t="inlineStr">
+        <is>
+          <t>UpfrontFeePayment_Comment</t>
+        </is>
+      </c>
+      <c r="G1" s="96" t="inlineStr">
+        <is>
+          <t>Borrower_ShortName</t>
+        </is>
+      </c>
+      <c r="H1" s="96" t="inlineStr">
+        <is>
+          <t>Lender_ShortName</t>
+        </is>
+      </c>
+      <c r="I1" s="96" t="inlineStr">
+        <is>
+          <t>Remittance_Instruction</t>
+        </is>
+      </c>
+      <c r="J1" s="96" t="inlineStr">
+        <is>
+          <t>Remittance_Description</t>
+        </is>
+      </c>
+      <c r="K1" s="101" t="inlineStr">
         <is>
           <t>Loan_Currency</t>
         </is>
       </c>
-      <c r="P1" s="29" t="inlineStr">
-        <is>
-          <t>Loan_RequestedAmount</t>
-        </is>
-      </c>
-      <c r="Q1" s="29" t="inlineStr">
-        <is>
-          <t>HostBankSharePct</t>
-        </is>
-      </c>
-      <c r="R1" s="30" t="inlineStr">
-        <is>
-          <t>Loan_EffectiveDate</t>
-        </is>
-      </c>
-      <c r="S1" s="30" t="inlineStr">
-        <is>
-          <t>Loan_MaturityDate</t>
-        </is>
-      </c>
-      <c r="T1" s="29" t="inlineStr">
-        <is>
-          <t>Loan_RepricingFrequency</t>
-        </is>
-      </c>
-      <c r="U1" s="29" t="inlineStr">
-        <is>
-          <t>Loan_IntCycleFrequency</t>
-        </is>
-      </c>
-      <c r="V1" s="29" t="inlineStr">
-        <is>
-          <t>Loan_Accrue</t>
-        </is>
-      </c>
-      <c r="W1" s="29" t="inlineStr">
-        <is>
-          <t>Borrower_BaseRate</t>
-        </is>
-      </c>
-      <c r="X1" s="29" t="inlineStr">
-        <is>
-          <t>Repayment_ScheduleFrequency</t>
-        </is>
-      </c>
-      <c r="Y1" s="29" t="inlineStr">
-        <is>
-          <t>Repayment_NumberOfCycles</t>
-        </is>
-      </c>
-      <c r="Z1" s="30" t="inlineStr">
-        <is>
-          <t>Repayment_TriggerDate</t>
-        </is>
-      </c>
-      <c r="AA1" s="29" t="inlineStr">
-        <is>
-          <t>Repayment_NonBusDayRule</t>
-        </is>
-      </c>
-      <c r="AB1" s="2" t="inlineStr">
-        <is>
-          <t>WIP_TransactionType</t>
-        </is>
-      </c>
-      <c r="AC1" s="2" t="inlineStr">
-        <is>
-          <t>WIP_AwaitingApprovalStatus</t>
-        </is>
-      </c>
-      <c r="AD1" s="2" t="inlineStr">
-        <is>
-          <t>WIP_OutstandingType</t>
-        </is>
-      </c>
-      <c r="AE1" s="2" t="inlineStr">
-        <is>
-          <t>WIP_AwaitingRateApprovalStatus</t>
-        </is>
-      </c>
-      <c r="AF1" s="2" t="inlineStr">
-        <is>
-          <t>WIP_AwaitingReleaseCashflowsStatus</t>
-        </is>
-      </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="L1" s="101" t="inlineStr">
+        <is>
+          <t>Remittance_Status</t>
+        </is>
+      </c>
+      <c r="M1" s="101" t="inlineStr">
         <is>
           <t>Borrower_Profile</t>
         </is>
       </c>
-      <c r="AH1" s="13" t="inlineStr">
-        <is>
-          <t>LIQCustomer_ShortName</t>
-        </is>
-      </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="N1" s="101" t="inlineStr">
         <is>
           <t>LIQCustomer_ID</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
-        <is>
-          <t>Remittance_Instruction</t>
-        </is>
-      </c>
-      <c r="AK1" s="2" t="inlineStr">
-        <is>
-          <t>Remittance_Status</t>
-        </is>
-      </c>
-      <c r="AL1" s="2" t="inlineStr">
-        <is>
-          <t>Loan_Currency</t>
-        </is>
-      </c>
-      <c r="AM1" s="13" t="inlineStr">
-        <is>
-          <t>Remittance_Description</t>
-        </is>
-      </c>
-      <c r="AN1" s="2" t="inlineStr">
-        <is>
-          <t>HostBank_GLAccount</t>
-        </is>
-      </c>
-      <c r="AO1" s="2" t="inlineStr">
-        <is>
-          <t>Borrower_GLAccount</t>
-        </is>
-      </c>
-      <c r="AP1" s="2" t="inlineStr">
-        <is>
-          <t>Host_Bank</t>
-        </is>
-      </c>
-      <c r="AQ1" s="2" t="inlineStr">
-        <is>
-          <t>NoticeStatus</t>
-        </is>
-      </c>
-      <c r="AR1" s="2" t="inlineStr">
-        <is>
-          <t>BranchCode</t>
+      <c r="O1" s="101" t="inlineStr">
+        <is>
+          <t>UpfrontFeePayment_NoticeMethod</t>
+        </is>
+      </c>
+      <c r="P1" s="102" t="inlineStr">
+        <is>
+          <t>Entity</t>
         </is>
       </c>
     </row>
-    <row r="2" customFormat="1" s="86">
-      <c r="A2" s="86" t="inlineStr">
+    <row r="2" ht="15" customFormat="1" customHeight="1" s="98">
+      <c r="A2" s="14" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="86" t="inlineStr">
-        <is>
-          <t>EVG_PTYLIQ01 Scenario1 Baseline Bilateral</t>
-        </is>
-      </c>
-      <c r="C2" s="31" t="inlineStr">
-        <is>
-          <t>john.blogg@abc.com</t>
-        </is>
-      </c>
-      <c r="D2" s="86" t="inlineStr">
+      <c r="B2" s="98" t="inlineStr">
+        <is>
+          <t>EVG_PTYLIQ04 Scenario4 Baseline Non Agent Syndication</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>NON RPA HB BRANCH 20M_20102020150220NIP</t>
         </is>
       </c>
-      <c r="E2" s="15" t="inlineStr">
+      <c r="D2" s="84" t="inlineStr">
+        <is>
+          <t>50,000</t>
+        </is>
+      </c>
+      <c r="E2" s="98" t="inlineStr">
+        <is>
+          <t>Establishment/Extension Fee</t>
+        </is>
+      </c>
+      <c r="F2" s="98" t="inlineStr">
+        <is>
+          <t>Upfront Fee Payment Transaction</t>
+        </is>
+      </c>
+      <c r="H2" s="86" t="inlineStr">
+        <is>
+          <t>CBA AMSTERDAM</t>
+        </is>
+      </c>
+      <c r="I2" s="98" t="inlineStr">
+        <is>
+          <t>IMT</t>
+        </is>
+      </c>
+      <c r="J2" s="98" t="inlineStr">
+        <is>
+          <t>IMT1</t>
+        </is>
+      </c>
+      <c r="K2" s="103" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="F2" s="86" t="inlineStr">
-        <is>
-          <t>CEU_FAC_10062020130642XHO</t>
-        </is>
-      </c>
-      <c r="G2" s="15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H2" s="86" t="inlineStr">
-        <is>
-          <t>100,000.00</t>
-        </is>
-      </c>
-      <c r="I2" s="86" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="J2" s="86" t="inlineStr">
-        <is>
-          <t>SHORTNME2255</t>
-        </is>
-      </c>
-      <c r="K2" s="15" t="inlineStr">
-        <is>
-          <t>Loan</t>
-        </is>
-      </c>
-      <c r="L2" s="86" t="inlineStr">
-        <is>
-          <t>CEU_FAC_10062020130642XHO</t>
-        </is>
-      </c>
-      <c r="M2" s="86" t="inlineStr">
-        <is>
-          <t>60000278</t>
-        </is>
-      </c>
-      <c r="N2" s="15" t="inlineStr">
-        <is>
-          <t>Fixed Rate Option</t>
-        </is>
-      </c>
-      <c r="O2" s="15" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="P2" s="15" t="inlineStr">
-        <is>
-          <t>10000.00</t>
-        </is>
-      </c>
-      <c r="Q2" s="15" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="R2" s="86" t="inlineStr">
-        <is>
-          <t>25-May-2020</t>
-        </is>
-      </c>
-      <c r="S2" s="86" t="inlineStr">
-        <is>
-          <t>26-May-2025</t>
-        </is>
-      </c>
-      <c r="T2" s="15" t="inlineStr">
-        <is>
-          <t>Monthly</t>
-        </is>
-      </c>
-      <c r="U2" s="15" t="inlineStr">
-        <is>
-          <t>Monthly</t>
-        </is>
-      </c>
-      <c r="V2" s="15" t="inlineStr">
-        <is>
-          <t>to the actual due date</t>
-        </is>
-      </c>
-      <c r="W2" s="15" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="X2" s="15" t="inlineStr">
-        <is>
-          <t>Weeks</t>
-        </is>
-      </c>
-      <c r="Y2" s="15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Z2" s="86" t="inlineStr">
-        <is>
-          <t>25-May-2020</t>
-        </is>
-      </c>
-      <c r="AA2" s="15" t="inlineStr">
-        <is>
-          <t>Next Business Day</t>
-        </is>
-      </c>
-      <c r="AB2" s="86" t="inlineStr">
-        <is>
-          <t>Outstandings</t>
-        </is>
-      </c>
-      <c r="AC2" s="86" t="inlineStr">
-        <is>
-          <t>Awaiting Approval</t>
-        </is>
-      </c>
-      <c r="AD2" s="86" t="inlineStr">
-        <is>
-          <t>Loan Initial Drawdown</t>
-        </is>
-      </c>
-      <c r="AE2" s="15" t="inlineStr">
-        <is>
-          <t>Awaiting Rate Approval</t>
-        </is>
-      </c>
-      <c r="AF2" s="15" t="inlineStr">
-        <is>
-          <t>Awaiting Release Cashflows</t>
-        </is>
-      </c>
-      <c r="AG2" s="15" t="inlineStr">
+      <c r="L2" s="103" t="inlineStr">
+        <is>
+          <t>DOIT</t>
+        </is>
+      </c>
+      <c r="M2" s="103" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="AH2" s="86" t="inlineStr">
-        <is>
-          <t>SHORTNME2255</t>
-        </is>
-      </c>
-      <c r="AI2" s="86" t="inlineStr">
-        <is>
-          <t>195</t>
-        </is>
-      </c>
-      <c r="AJ2" s="86" t="inlineStr">
-        <is>
-          <t>IMT</t>
-        </is>
-      </c>
-      <c r="AK2" s="86" t="inlineStr">
-        <is>
-          <t>DOIT</t>
-        </is>
-      </c>
-      <c r="AL2" s="86" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="AM2" s="86" t="inlineStr">
-        <is>
-          <t>IMTEUR1-0902</t>
-        </is>
-      </c>
-      <c r="AN2" s="32" t="inlineStr">
-        <is>
-          <t>12001001836</t>
-        </is>
-      </c>
-      <c r="AO2" s="32" t="inlineStr">
-        <is>
-          <t>18567000000</t>
-        </is>
-      </c>
-      <c r="AP2" s="86" t="inlineStr">
-        <is>
-          <t>CG852/Hold for Investment - Europe/BP_CML</t>
-        </is>
-      </c>
-      <c r="AQ2" s="86" t="inlineStr">
-        <is>
-          <t>Awaiting release</t>
-        </is>
-      </c>
-      <c r="AR2" s="86" t="inlineStr">
-        <is>
-          <t>CG852</t>
+      <c r="N2" s="103" t="n">
+        <v>35</v>
+      </c>
+      <c r="O2" s="103" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="P2" s="104" t="inlineStr">
+        <is>
+          <t>EU</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="AP5" s="33" t="n"/>
+    <row r="10">
+      <c r="M10" s="99" t="n"/>
+      <c r="R10" s="100" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
GDE-8212 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S4_EU_NonRPA_Branch.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S4_EU_NonRPA_Branch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D0C36E-8BBA-4AE1-97B9-0C5EBD42A52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4893136A-76EC-48AB-9155-EC496CBF4DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="923" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <sheet name="CRED08_OngoingFeeSetup" sheetId="7" r:id="rId7"/>
     <sheet name="SYND02_PrimaryAllocation" sheetId="8" r:id="rId8"/>
     <sheet name="CRED07_UpfrontFee_Payment" sheetId="9" r:id="rId9"/>
-    <sheet name="SERV01_LoanDrawdown" sheetId="10" r:id="rId10"/>
-    <sheet name="AMCH06_PricingChangeTransaction" sheetId="11" r:id="rId11"/>
-    <sheet name="DLCH01_DealChangeTransaction" sheetId="12" r:id="rId12"/>
-    <sheet name="SERV18_Payments" sheetId="13" r:id="rId13"/>
-    <sheet name="SERV21_InterestPayments" sheetId="14" r:id="rId14"/>
-    <sheet name="SERV29_PaymentFees" sheetId="15" r:id="rId15"/>
-    <sheet name="AMCH04_DealChangeTransaction" sheetId="16" r:id="rId16"/>
-    <sheet name="TRPO12_PortfolioSettledDisc" sheetId="17" r:id="rId17"/>
+    <sheet name="TRPO12_PortfolioSettledDisc" sheetId="17" r:id="rId10"/>
+    <sheet name="SERV01_LoanDrawdown" sheetId="10" r:id="rId11"/>
+    <sheet name="AMCH06_PricingChangeTransaction" sheetId="11" r:id="rId12"/>
+    <sheet name="DLCH01_DealChangeTransaction" sheetId="12" r:id="rId13"/>
+    <sheet name="SERV18_Payments" sheetId="13" r:id="rId14"/>
+    <sheet name="SERV21_InterestPayments" sheetId="14" r:id="rId15"/>
+    <sheet name="SERV29_PaymentFees" sheetId="15" r:id="rId16"/>
+    <sheet name="AMCH04_DealChangeTransaction" sheetId="16" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="873">
   <si>
     <t>rowid</t>
   </si>
@@ -2649,55 +2649,25 @@
     <t>Short_Name</t>
   </si>
   <si>
-    <t>Transaction_Type</t>
-  </si>
-  <si>
-    <t>Transaction_Status_Awaiting_Approval</t>
-  </si>
-  <si>
-    <t>Payment_Type</t>
-  </si>
-  <si>
-    <t>Transaction_Status_Awaiting_Release</t>
-  </si>
-  <si>
     <t>Portfolio_Position</t>
   </si>
   <si>
-    <t>Adjustment_Amount</t>
-  </si>
-  <si>
     <t>GL_ShortName</t>
   </si>
   <si>
-    <t>AwaitingDispose</t>
-  </si>
-  <si>
-    <t>PFDC_Transaction_Type</t>
-  </si>
-  <si>
-    <t>PFDC_Payment_Type</t>
-  </si>
-  <si>
-    <t>Fee Payment From Borrower</t>
-  </si>
-  <si>
-    <t>Awaiting Release</t>
-  </si>
-  <si>
-    <t>Interest Income</t>
-  </si>
-  <si>
-    <t>BNS1_02052020132235LFZ</t>
-  </si>
-  <si>
-    <t>Facilities</t>
-  </si>
-  <si>
-    <t>Portfolio Settled Discount Adjustment</t>
-  </si>
-  <si>
     <t>IMT1</t>
+  </si>
+  <si>
+    <t>Fees Held Awaiting Dispos.</t>
+  </si>
+  <si>
+    <t>GL_Offset_Type</t>
+  </si>
+  <si>
+    <t>Existing WIP</t>
+  </si>
+  <si>
+    <t>Portfolio_Name</t>
   </si>
 </sst>
 </file>
@@ -2965,7 +2935,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3098,8 +3068,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3881,6 +3849,103 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="88" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="88" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="88" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="88" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="88" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="88" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" style="88" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" style="88" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="88" customWidth="1"/>
+    <col min="10" max="17" width="8.7109375" style="88" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="88"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>421</v>
+      </c>
+      <c r="E1" s="87" t="s">
+        <v>865</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>872</v>
+      </c>
+      <c r="G1" s="91" t="s">
+        <v>866</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>867</v>
+      </c>
+      <c r="I1" s="89" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>645</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>515</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>517</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" s="86" t="s">
+        <v>650</v>
+      </c>
+      <c r="G2" s="86"/>
+      <c r="H2" s="88" t="s">
+        <v>869</v>
+      </c>
+      <c r="I2" s="88" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="46"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4216,7 +4281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4530,7 +4595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4596,7 +4661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4944,7 +5009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5284,7 +5349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5592,7 +5657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5657,134 +5722,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.85546875" style="88" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="88" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44" style="88" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" style="88" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.7109375" style="88" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="88" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="88" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="88" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="88" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" style="88" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" style="88" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="8.7109375" style="88" customWidth="1"/>
-    <col min="24" max="16384" width="8.7109375" style="88"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="89" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="92" t="s">
-        <v>419</v>
-      </c>
-      <c r="D1" s="92" t="s">
-        <v>421</v>
-      </c>
-      <c r="E1" s="87" t="s">
-        <v>865</v>
-      </c>
-      <c r="F1" s="87" t="s">
-        <v>866</v>
-      </c>
-      <c r="G1" s="87" t="s">
-        <v>867</v>
-      </c>
-      <c r="H1" s="87" t="s">
-        <v>868</v>
-      </c>
-      <c r="I1" s="87" t="s">
-        <v>869</v>
-      </c>
-      <c r="J1" s="93" t="s">
-        <v>870</v>
-      </c>
-      <c r="K1" s="89" t="s">
-        <v>871</v>
-      </c>
-      <c r="L1" s="89" t="s">
-        <v>872</v>
-      </c>
-      <c r="M1" s="89" t="s">
-        <v>873</v>
-      </c>
-      <c r="N1" s="89" t="s">
-        <v>874</v>
-      </c>
-      <c r="O1" s="89" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="86" t="s">
-        <v>645</v>
-      </c>
-      <c r="C2" s="86" t="s">
-        <v>515</v>
-      </c>
-      <c r="D2" s="86" t="s">
-        <v>517</v>
-      </c>
-      <c r="E2" s="86" t="s">
-        <v>306</v>
-      </c>
-      <c r="F2" s="86" t="s">
-        <v>833</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>876</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>877</v>
-      </c>
-      <c r="J2" s="86" t="s">
-        <v>517</v>
-      </c>
-      <c r="K2" s="90">
-        <v>4000</v>
-      </c>
-      <c r="L2" s="88" t="s">
-        <v>878</v>
-      </c>
-      <c r="M2" s="91" t="s">
-        <v>879</v>
-      </c>
-      <c r="N2" s="88" t="s">
-        <v>880</v>
-      </c>
-      <c r="O2" s="88" t="s">
-        <v>881</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -8739,8 +8676,8 @@
   <dimension ref="A1:AQ4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z2" sqref="Z2"/>
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8884,13 +8821,13 @@
       <c r="AE1" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="AF1" s="94" t="s">
+      <c r="AF1" s="92" t="s">
         <v>637</v>
       </c>
-      <c r="AG1" s="94" t="s">
+      <c r="AG1" s="92" t="s">
         <v>198</v>
       </c>
-      <c r="AH1" s="95" t="s">
+      <c r="AH1" s="93" t="s">
         <v>507</v>
       </c>
       <c r="AI1" s="2" t="s">
@@ -8902,7 +8839,7 @@
       <c r="AK1" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="AL1" s="94" t="s">
+      <c r="AL1" s="92" t="s">
         <v>625</v>
       </c>
       <c r="AM1" s="2" t="s">
@@ -9090,42 +9027,42 @@
   </sheetPr>
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="98" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52" style="98" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" style="98" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="98" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="98" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="98" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" style="98" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" style="98" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="98" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="98" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" style="98" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="98" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" style="98" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="96" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52" style="96" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="96" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" style="96" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="96" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="96" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="96" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="96" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="96" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="96" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="96" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" style="96" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="97" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="95" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="94" t="s">
         <v>419</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="94" t="s">
         <v>449</v>
       </c>
       <c r="E1" s="24" t="s">
@@ -9134,45 +9071,45 @@
       <c r="F1" s="24" t="s">
         <v>661</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="94" t="s">
         <v>662</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="94" t="s">
         <v>663</v>
       </c>
-      <c r="I1" s="96" t="s">
+      <c r="I1" s="94" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="96" t="s">
+      <c r="J1" s="94" t="s">
         <v>664</v>
       </c>
-      <c r="K1" s="101" t="s">
+      <c r="K1" s="99" t="s">
         <v>665</v>
       </c>
-      <c r="L1" s="101" t="s">
+      <c r="L1" s="99" t="s">
         <v>666</v>
       </c>
-      <c r="M1" s="101" t="s">
+      <c r="M1" s="99" t="s">
         <v>667</v>
       </c>
-      <c r="N1" s="101" t="s">
+      <c r="N1" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="O1" s="101" t="s">
+      <c r="O1" s="99" t="s">
         <v>668</v>
       </c>
-      <c r="P1" s="102" t="s">
+      <c r="P1" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="Q1" s="96" t="s">
+      <c r="Q1" s="94" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="98" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="96" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="96" t="s">
         <v>670</v>
       </c>
       <c r="C2" t="s">
@@ -9181,44 +9118,44 @@
       <c r="D2" s="84" t="s">
         <v>550</v>
       </c>
-      <c r="E2" s="98" t="s">
+      <c r="E2" s="96" t="s">
         <v>548</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="96" t="s">
         <v>671</v>
       </c>
       <c r="H2" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="96" t="s">
         <v>300</v>
       </c>
-      <c r="J2" s="98" t="s">
-        <v>882</v>
-      </c>
-      <c r="K2" s="103" t="s">
+      <c r="J2" s="96" t="s">
+        <v>868</v>
+      </c>
+      <c r="K2" s="101" t="s">
         <v>310</v>
       </c>
-      <c r="L2" s="103" t="s">
+      <c r="L2" s="101" t="s">
         <v>672</v>
       </c>
-      <c r="M2" s="103" t="s">
+      <c r="M2" s="101" t="s">
         <v>322</v>
       </c>
-      <c r="N2" s="103">
+      <c r="N2" s="101">
         <v>35</v>
       </c>
-      <c r="O2" s="103" t="s">
+      <c r="O2" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="104" t="s">
+      <c r="P2" s="102" t="s">
         <v>392</v>
       </c>
       <c r="Q2" s="86"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="M10" s="99"/>
-      <c r="R10" s="100"/>
+      <c r="M10" s="97"/>
+      <c r="R10" s="98"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
GDE-8219 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S4_EU_NonRPA_Branch.xlsx
+++ b/DataSet/LoanIQ_DataSet/EU_Entity/EVG_S4_EU_NonRPA_Branch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\EU_Entity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0838A011-5F7E-47A0-A92B-93DB37FA9C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D429FD6-3A59-4493-8EB4-6239173492B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="923" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="873">
   <si>
     <t>rowid</t>
   </si>
@@ -2663,6 +2663,12 @@
   </si>
   <si>
     <t>Borrower1_RemittanceInstruction</t>
+  </si>
+  <si>
+    <t>Facility_FeeMatrixMethod</t>
+  </si>
+  <si>
+    <t>Utilized</t>
   </si>
 </sst>
 </file>
@@ -4304,8 +4310,8 @@
   </sheetPr>
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8605,13 +8611,13 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V1:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8634,9 +8640,10 @@
     <col min="18" max="19" width="21" style="86" customWidth="1"/>
     <col min="20" max="20" width="22" style="86" customWidth="1"/>
     <col min="21" max="21" width="25.42578125" style="86" customWidth="1"/>
+    <col min="22" max="22" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -8700,8 +8707,11 @@
       <c r="U1" s="2" t="s">
         <v>606</v>
       </c>
+      <c r="V1" s="2" t="s">
+        <v>871</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
         <v>48</v>
       </c>
@@ -8765,8 +8775,11 @@
       <c r="U2" s="86" t="s">
         <v>618</v>
       </c>
+      <c r="V2" s="86" t="s">
+        <v>872</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="46"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -8782,7 +8795,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="46"/>
     </row>
-    <row r="4" spans="1:21" s="86" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>

</xml_diff>